<commit_message>
RiskList - Aktualizace kategorii a vysvětlivek
Dodal jsem vysvětlivky a poupravil kategorie listu.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Files\Ostravská univerzita\Magisterské studium\Předměty\1. Semestr\7RPR1\Projekty\EuroKlíčenka 2.0\Repozitář\RPR1\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D7566-B5FE-4A92-8FDE-95B24120481B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F79DCB-AFD0-41F8-A850-284D4C55FE80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Risk</t>
   </si>
@@ -46,36 +46,12 @@
     <t>Pravděpodobnost</t>
   </si>
   <si>
-    <t>Vliv</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Položky</t>
-  </si>
-  <si>
     <t>MA (Mitigační akce)</t>
   </si>
   <si>
     <t>Ztráta přehledu</t>
   </si>
   <si>
-    <t>Vysoký</t>
-  </si>
-  <si>
     <t>Trakování veškeré aktivity v Jire. Pravidelné updaty v MS Teams.</t>
   </si>
   <si>
@@ -88,18 +64,12 @@
     <t>Vyjasnění situace s konzultantem.</t>
   </si>
   <si>
-    <t>Podpora pro IOS</t>
-  </si>
-  <si>
     <t>Neznalost architektury</t>
   </si>
   <si>
     <t>Bez známosti použité architektury není možné začít vývoj projektu.</t>
   </si>
   <si>
-    <t>vysoký</t>
-  </si>
-  <si>
     <t>Provnat možné existující architektury =&gt; vytvořit dokument popisující možnou použitou. Vytvořit prototyp.</t>
   </si>
   <si>
@@ -107,13 +77,40 @@
   </si>
   <si>
     <t>EuroKlíčenka 2.0 - RiskList</t>
+  </si>
+  <si>
+    <t>Priorita</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Co to je za druh risku.</t>
+  </si>
+  <si>
+    <t>Jak ovlivní následující vývoj projektu</t>
+  </si>
+  <si>
+    <t>Jak moc je daný risk brán v úvahu v tento čas/jak moc se s ním právě počítá</t>
+  </si>
+  <si>
+    <t>Možné provedilné akce, snižující šanci nastání risku</t>
+  </si>
+  <si>
+    <t>Jak vysoká je šance, že risk projekt ohrozí v tuto dobu.</t>
+  </si>
+  <si>
+    <t>Podpora pro iOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,14 +137,6 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="8" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
@@ -200,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,8 +223,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -349,19 +344,6 @@
         <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right/>
-      <top style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
       <top style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </top>
@@ -434,38 +416,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="0.39994506668294322"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -487,30 +552,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="6" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hypertextový odkaz" xfId="4" builtinId="8"/>
@@ -519,10 +611,10 @@
     <cellStyle name="Správně" xfId="1" builtinId="26"/>
     <cellStyle name="Špatně" xfId="2" builtinId="27"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="12">
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -540,9 +632,46 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <left/>
+        <right style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
-        </left>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right/>
         <top style="thin">
           <color theme="1" tint="0.34998626667073579"/>
@@ -570,7 +699,7 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -629,11 +758,107 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
         </right>
@@ -692,174 +917,13 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
         </left>
         <right style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
         </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.24994659260841701"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
         <top/>
         <bottom/>
       </border>
@@ -922,15 +986,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G8" headerRowDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G8" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B3:G8" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{72B2E65B-D615-42C2-9AAE-33E400E5293A}" name="Položky" totalsRowLabel="Celkem" dataDxfId="9" totalsRowDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{BC20C5C9-5919-4826-A623-300689436274}" name="Risk" dataDxfId="7" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0C8BAE52-5BE6-4F40-BB1E-DB32549DF409}" name="Dopad" dataDxfId="5" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8A33ED25-90FD-4225-9B0A-D74C7E54E6CD}" name="Pravděpodobnost" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8D4061F9-96CF-4B77-9653-49FCDCF301F4}" name="Vliv" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{B3C5C666-1EB6-4DC5-ABA1-16D42A2B0116}" name="MA (Mitigační akce)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{72B2E65B-D615-42C2-9AAE-33E400E5293A}" name="ID" totalsRowLabel="Celkem" dataDxfId="1">
+      <calculatedColumnFormula>"R"&amp;ROW($A1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{BC20C5C9-5919-4826-A623-300689436274}" name="Risk" dataDxfId="0" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{0C8BAE52-5BE6-4F40-BB1E-DB32549DF409}" name="Dopad" dataDxfId="7" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{B3C5C666-1EB6-4DC5-ABA1-16D42A2B0116}" name="MA (Mitigační akce)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{8D4061F9-96CF-4B77-9653-49FCDCF301F4}" name="Priorita" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8A33ED25-90FD-4225-9B0A-D74C7E54E6CD}" name="Pravděpodobnost" dataDxfId="4" totalsRowDxfId="5" dataCellStyle="Správně"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1199,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:K33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,26 +1277,31 @@
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+    <row r="1" spans="2:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="2:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
-        <v>9</v>
+    <row r="3" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -1239,106 +1310,143 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="str">
+        <f t="shared" ref="B4:B8" si="0">"R"&amp;ROW($A1)</f>
+        <v>R1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="20">
+        <v>5</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>R2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="20">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>R3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="20">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
+      <c r="G6" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>13</v>
+    <row r="7" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>R4</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="J7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="19">
-        <v>0.75</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="22" t="s">
-        <v>22</v>
-      </c>
+    <row r="8" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>R5</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
-    <row r="6" spans="2:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="2:8" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1357,9 +1465,9 @@
     <row r="32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" xr:uid="{DA384BF8-56CD-43AC-9705-4603A93A457B}"/>
+    <hyperlink ref="H5" r:id="rId1" xr:uid="{4F76D589-BBB3-407C-8F79-8A574AA13CB0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Test nahrání projektu EuroKlíčenka
1. Zkouška nahrání projektu euroklíčenka.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ondrej\Documents\GitHub\RPR1\Dokumenty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EuroKlíčenka 2.0\RPR1\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124DDFCE-AF76-4796-91C8-864F2E78EF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF704D77-096A-4382-A6E1-001F4E3B85A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,20 +128,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -222,7 +214,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,20 +254,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -551,68 +531,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -627,29 +632,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="8" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="6" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="8" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1315,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1356,7 @@
       <c r="G2" s="16"/>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1366,10 +1374,10 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="21" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1387,16 +1395,16 @@
       <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="31">
         <v>5</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="24">
         <v>0.25</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="22" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1414,7 +1422,7 @@
       <c r="E5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="32">
         <v>4</v>
       </c>
       <c r="G5" s="11">
@@ -1423,10 +1431,10 @@
       <c r="H5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1444,16 +1452,16 @@
       <c r="E6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="32">
         <v>3</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>0.5</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1465,7 +1473,7 @@
       <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1474,13 +1482,13 @@
       <c r="F7" s="2">
         <v>5</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="29">
         <v>0.5</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="23" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1501,11 +1509,11 @@
       <c r="F8" s="3">
         <v>5</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="30">
         <v>0.25</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
     </row>
     <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1533,7 +1541,7 @@
     <row r="32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H5" r:id="rId1" xr:uid="{4F76D589-BBB3-407C-8F79-8A574AA13CB0}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Aktualizace RiskListu + Pořádek v repu
Aktualizoval jsem RiskList dle připomínek z poslední schůzky. Zároveň jsem hodil Kotlin prototyp EUK2 do své vlastní složky.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EUK2\RPR1\Dokumenty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EUK2\RPR-Repo\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AF84A6-C92C-4C52-975E-31E4A2E9BE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83261AC-A471-46D4-BB7D-6DF4B242FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Risk</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Členové týmu nebudou na stejné stránce, ohledně stavu projektu. Může dojít k nevědomosti, co už je hotové a co je třeba udělat dál.</t>
   </si>
   <si>
-    <t>Bylo by nutné úplně změnit použitou architekturu, po případě vytvořit 2. aplikaci.</t>
-  </si>
-  <si>
-    <t>Vyjasnění situace s konzultantem.</t>
-  </si>
-  <si>
     <t>Neznalost architektury</t>
   </si>
   <si>
@@ -89,30 +83,18 @@
     <t>Možné provedilné akce, snižující šanci nastání risku</t>
   </si>
   <si>
-    <t>Podpora pro iOS</t>
-  </si>
-  <si>
     <t>Nekvalitní kód</t>
   </si>
   <si>
     <t>Rychle psaný a nekontrolovaný kód vede ke slabé udržitelnosti a snížené použitelnosti (bugy) softwaru.</t>
   </si>
   <si>
-    <t>Náhlé změny cílů projektu</t>
-  </si>
-  <si>
     <t>Promarněný čas, nekompletní funkce.</t>
   </si>
   <si>
-    <t>Porovnat možné existující architektury =&gt; vytvořit dokument popisující možnou použitou. Vytvořit prototyp.</t>
-  </si>
-  <si>
     <t>Slabá komunikace</t>
   </si>
   <si>
-    <t>Trakování prováděné aktivity v Jire. Pravidelné updaty a souhrny v MS Teams.</t>
-  </si>
-  <si>
     <t>Ztráta člena týmu</t>
   </si>
   <si>
@@ -122,13 +104,22 @@
     <t>Snížení efektivnosti celého týmu a zvýšení zátěže pro zbývající členy.</t>
   </si>
   <si>
-    <t>Častá komunikace mezi jednotlivými členy. Alespoň 2 členové týmu se orientují v dané oblasti.</t>
-  </si>
-  <si>
-    <t>Jasná vize (dokument), stabilní architektura.</t>
-  </si>
-  <si>
-    <t>Průběžné testování.</t>
+    <t>Sledování prováděné aktivity v Jire. Přidělení práce hned na začátku sprintu. Kontrola před koncem. O nečekaných změnách ohledně práce informovat celý tým několik dní předem.</t>
+  </si>
+  <si>
+    <t>Porovnat vhodné architektury, vybrat tu, která splňuje nejvíc požadavků. Seznámit se s jejími funkcemi vytvořením drobného prototypu.</t>
+  </si>
+  <si>
+    <t>Častá komunikace mezi jednotlivými členy. Dokumentace prováděné činnosti (např XML komentáře).</t>
+  </si>
+  <si>
+    <t>Náhlé změny požadavků (zákazníkem)</t>
+  </si>
+  <si>
+    <t>Průběžné manuální testování. Příprava automatických testů.</t>
+  </si>
+  <si>
+    <t>Domluva se zákazníkem =&gt; Způsob "Něco za něco" - implementace funkcí na úkor jiných.</t>
   </si>
 </sst>
 </file>
@@ -242,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -422,28 +413,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color theme="1" tint="0.34998626667073579"/>
       </top>
       <bottom style="thin">
@@ -456,42 +447,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -499,186 +456,147 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
+      <top style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right style="medium">
-        <color theme="1" tint="0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
       </bottom>
       <diagonal/>
     </border>
@@ -689,7 +607,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -733,71 +651,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="25" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="25" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="5" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="5" borderId="32" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="5" borderId="30" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -807,80 +710,6 @@
     <cellStyle name="Špatně" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="1" tint="0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -908,6 +737,45 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -1109,6 +977,41 @@
         <charset val="238"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="1" tint="0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -1189,17 +1092,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G9" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="B3:G9" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G8" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="B3:G8" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72B2E65B-D615-42C2-9AAE-33E400E5293A}" name="ID" totalsRowLabel="Celkem" dataDxfId="9">
       <calculatedColumnFormula>"R"&amp;ROW($A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{BC20C5C9-5919-4826-A623-300689436274}" name="Risk" dataDxfId="1" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0C8BAE52-5BE6-4F40-BB1E-DB32549DF409}" name="Dopad" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{B3C5C666-1EB6-4DC5-ABA1-16D42A2B0116}" name="MA (Mitigační akce)" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{8D4061F9-96CF-4B77-9653-49FCDCF301F4}" name="Priorita" totalsRowFunction="count" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8A33ED25-90FD-4225-9B0A-D74C7E54E6CD}" name="Pravděpodobnost" dataDxfId="0" totalsRowDxfId="2" dataCellStyle="Správně"/>
+    <tableColumn id="2" xr3:uid="{BC20C5C9-5919-4826-A623-300689436274}" name="Risk" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0C8BAE52-5BE6-4F40-BB1E-DB32549DF409}" name="Dopad" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{B3C5C666-1EB6-4DC5-ABA1-16D42A2B0116}" name="MA (Mitigační akce)" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{8D4061F9-96CF-4B77-9653-49FCDCF301F4}" name="Priorita" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8A33ED25-90FD-4225-9B0A-D74C7E54E6CD}" name="Pravděpodobnost" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1468,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K31"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,8 +1386,8 @@
     <col min="5" max="5" width="36.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" customWidth="1"/>
+    <col min="9" max="9" width="63" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" customWidth="1"/>
@@ -1494,7 +1397,7 @@
     <row r="1" spans="2:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1504,7 +1407,7 @@
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -1516,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -1525,34 +1428,34 @@
         <v>0</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="str">
         <f>"R"&amp;ROW($A1)</f>
         <v>R1</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="29">
+      <c r="E4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="25">
         <v>5</v>
       </c>
-      <c r="G4" s="38">
-        <v>0.4</v>
+      <c r="G4" s="30">
+        <v>0.45</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1560,81 +1463,81 @@
         <f>"R"&amp;ROW($A2)</f>
         <v>R2</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>7</v>
+      <c r="C5" s="22" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="30">
-        <v>4</v>
-      </c>
-      <c r="G5" s="35">
-        <v>0.65</v>
+        <v>6</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="26">
+        <v>5</v>
+      </c>
+      <c r="G5" s="29">
+        <v>0.55000000000000004</v>
       </c>
       <c r="H5" s="3"/>
       <c r="J5" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>"R"&amp;ROW($A3)</f>
+        <f t="shared" ref="B6:B8" si="0">"R"&amp;ROW($A3)</f>
         <v>R3</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="31">
-        <v>4</v>
-      </c>
-      <c r="G6" s="36">
-        <v>0.5</v>
+      <c r="C6" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="27">
+        <v>2</v>
+      </c>
+      <c r="G6" s="28">
+        <v>0.75</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7:B9" si="0">"R"&amp;ROW($A4)</f>
+        <f t="shared" si="0"/>
         <v>R4</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="32">
-        <v>3</v>
-      </c>
-      <c r="G7" s="36">
-        <v>0.4</v>
+      <c r="C7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="33">
+        <v>5</v>
+      </c>
+      <c r="G7" s="28">
+        <v>0.75</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>2</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1642,45 +1545,25 @@
         <f t="shared" si="0"/>
         <v>R5</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>29</v>
+      <c r="E8" s="32" t="s">
+        <v>24</v>
       </c>
       <c r="F8" s="33">
-        <v>5</v>
-      </c>
-      <c r="G8" s="35">
-        <v>0.75</v>
+        <v>3</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0.5</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>R6</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="34">
-        <v>3</v>
-      </c>
-      <c r="G9" s="37">
-        <v>0.5</v>
-      </c>
-    </row>
+    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1577,7 @@
     <row r="20" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1702,7 +1585,6 @@
     <row r="28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Grafická úprava d. d. architektury
Jen jsem trochu graficky upravil náš demonstrační diagram architektury od Honzy Sonnka (odstranil grid-liny, aktor -> uživatel) a přesunul do složky Diagramy.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EUK2\RPR-Repo\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83261AC-A471-46D4-BB7D-6DF4B242FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16B4378-752C-469F-91DD-C83921235C90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>Porovnat vhodné architektury, vybrat tu, která splňuje nejvíc požadavků. Seznámit se s jejími funkcemi vytvořením drobného prototypu.</t>
   </si>
   <si>
-    <t>Častá komunikace mezi jednotlivými členy. Dokumentace prováděné činnosti (např XML komentáře).</t>
-  </si>
-  <si>
     <t>Náhlé změny požadavků (zákazníkem)</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Domluva se zákazníkem =&gt; Způsob "Něco za něco" - implementace funkcí na úkor jiných.</t>
+  </si>
+  <si>
+    <t>Častá komunikace mezi jednotlivými členy. Dokumentace prováděné činnosti (např XML komentáře v kódu).</t>
   </si>
 </sst>
 </file>
@@ -575,9 +575,11 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color theme="1" tint="0.34998626667073579"/>
       </right>
       <top style="thin">
         <color theme="1" tint="0.34998626667073579"/>
@@ -589,9 +591,11 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
       <top style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </top>
@@ -1371,10 +1375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K30"/>
+  <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1450,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="30">
         <v>0.45</v>
@@ -1488,7 +1492,7 @@
     </row>
     <row r="6" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B8" si="0">"R"&amp;ROW($A3)</f>
+        <f t="shared" ref="B6:B7" si="0">"R"&amp;ROW($A3)</f>
         <v>R3</v>
       </c>
       <c r="C6" s="23" t="s">
@@ -1498,7 +1502,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="27">
         <v>2</v>
@@ -1519,13 +1523,13 @@
         <v>R4</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="33">
         <v>5</v>
@@ -1542,7 +1546,7 @@
     </row>
     <row r="8" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>"R"&amp;ROW($A5)</f>
         <v>R5</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1552,7 +1556,7 @@
         <v>21</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F8" s="33">
         <v>3</v>
@@ -1575,16 +1579,14 @@
     <row r="18" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aktualizace RiskListu + odstranění nepořádku
V RiskListu jsem aktualizoval pravděpodobnosti a lépe specifikoval řešení pro R3.
Zároveň jsem odstranil balast z main.dart.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EUK2\RPR-Repo\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FC261C-717F-4555-B32A-2638950AA85C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF2368-EABD-47C0-AABE-83CD8A244C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,17 +116,17 @@
     <t>Domluva se zákazníkem =&gt; Způsob "Něco za něco" - implementace funkcí na úkor jiných.</t>
   </si>
   <si>
-    <t>Průběžné manuální testování. Tvorba automatických testů.</t>
-  </si>
-  <si>
     <t>Aspoň jeden další člen má přehled v problematice chybějící osoby. Dokumentace prováděné činnosti (např XML komentáře v kódu). Krátké sprinty (1-2 týdny).</t>
+  </si>
+  <si>
+    <t>Použití architektury (MVVM), dodržování best practises. Průběžné manuální testování. Tvorba automatických testů.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +196,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +240,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="28">
     <border>
@@ -605,11 +618,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -703,14 +717,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="5" borderId="24" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Hypertextový odkaz" xfId="3" builtinId="8"/>
     <cellStyle name="Neutrální" xfId="2" builtinId="28"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Správně" xfId="4" builtinId="26"/>
     <cellStyle name="Špatně" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="13">
@@ -1378,7 +1393,7 @@
   <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,7 +1468,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="33">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>1</v>
@@ -1502,7 +1517,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="27">
         <v>2</v>
@@ -1534,8 +1549,8 @@
       <c r="F7" s="32">
         <v>3</v>
       </c>
-      <c r="G7" s="28">
-        <v>0.75</v>
+      <c r="G7" s="29">
+        <v>0.55000000000000004</v>
       </c>
       <c r="J7" s="15" t="s">
         <v>2</v>
@@ -1556,7 +1571,7 @@
         <v>21</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="32">
         <v>3</v>

</xml_diff>

<commit_message>
RiskList - Nový Risk - načítání dat
* Dodal jsem nový risk, týkající se způsobu načítání dat.
* Zároveň jsem pravděpodobnosti.
</commit_message>
<xml_diff>
--- a/Dokumenty/RiskList.xlsx
+++ b/Dokumenty/RiskList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User\Projekty\School\EUK2\RPR-Repo\Dokumenty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF2368-EABD-47C0-AABE-83CD8A244C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF8972-4436-4845-B256-74108B2BAEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Risk</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Členové týmu nebudou na stejné stránce, ohledně stavu projektu. Může dojít k nevědomosti, co už je hotové a co je třeba udělat dál.</t>
   </si>
   <si>
-    <t>Neznalost architektury</t>
-  </si>
-  <si>
-    <t>Bez známosti použité architektury není možné začít vývoj projektu.</t>
-  </si>
-  <si>
     <t>EuroKlíčenka 2.0 - RiskList</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>Sledování prováděné aktivity v Jire. Přidělení práce hned na začátku sprintu. Kontrola před koncem. O nečekaných změnách ohledně práce informovat celý tým několik dní předem.</t>
   </si>
   <si>
-    <t>Porovnat vhodné architektury, vybrat tu, která splňuje nejvíc požadavků. Seznámit se s jejími funkcemi vytvořením drobného prototypu.</t>
-  </si>
-  <si>
     <t>Náhlé změny požadavků (zákazníkem)</t>
   </si>
   <si>
@@ -120,6 +111,24 @@
   </si>
   <si>
     <t>Použití architektury (MVVM), dodržování best practises. Průběžné manuální testování. Tvorba automatických testů.</t>
+  </si>
+  <si>
+    <t>Způsob načítání dat</t>
+  </si>
+  <si>
+    <t>Špatný způsob, jak data načítat povede k složité udržitelnosti a následovném rozšiřování databáze.</t>
+  </si>
+  <si>
+    <t>Neznalost technologie</t>
+  </si>
+  <si>
+    <t>Bez známosti použité technologie není možné začít vývoj projektu.</t>
+  </si>
+  <si>
+    <t>Porovnat vhodné technologie, vybrat tu, která splňuje nejvíc požadavků. Seznámit se s jejími součásmi vytvořením drobného prototypu.</t>
+  </si>
+  <si>
+    <t>Prozkoumat nejpoužívanější způsoby správy dat pro vybranou technologii. Zvolit tu pro projekt nejvhodnější.</t>
   </si>
 </sst>
 </file>
@@ -246,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -609,6 +618,32 @@
       <right style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right/>
       <top style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </top>
@@ -625,7 +660,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -719,6 +754,18 @@
     </xf>
     <xf numFmtId="9" fontId="9" fillId="7" borderId="24" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1111,8 +1158,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G8" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="B3:G8" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}" name="RiskList" displayName="RiskList" ref="B3:G9" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="B3:G9" xr:uid="{07D219B5-F8E7-49B9-9FB8-325B649B9EA2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72B2E65B-D615-42C2-9AAE-33E400E5293A}" name="ID" totalsRowLabel="Celkem" dataDxfId="9">
       <calculatedColumnFormula>"R"&amp;ROW($A1)</calculatedColumnFormula>
@@ -1392,8 +1439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="129" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="129" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1463,7 @@
     <row r="1" spans="2:11" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1426,7 +1473,7 @@
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -1438,7 +1485,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>2</v>
@@ -1447,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1456,13 +1503,13 @@
         <v>R1</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="25">
         <v>4</v>
@@ -1474,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1483,13 +1530,13 @@
         <v>R2</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F5" s="26">
         <v>5</v>
@@ -1499,10 +1546,10 @@
       </c>
       <c r="H5" s="3"/>
       <c r="J5" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1511,25 +1558,25 @@
         <v>R3</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" s="27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="28">
         <v>0.75</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="54.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1538,13 +1585,13 @@
         <v>R4</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="32">
         <v>3</v>
@@ -1556,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,13 +1612,13 @@
         <v>R5</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="30" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="31" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F8" s="32">
         <v>3</v>
@@ -1582,7 +1629,27 @@
       <c r="J8" s="8"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="str">
+        <f>"R"&amp;ROW($A6)</f>
+        <v>R6</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="37">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28">
+        <v>0.75</v>
+      </c>
+    </row>
     <row r="10" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:11" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>